<commit_message>
Added the required changes to finalize the build
</commit_message>
<xml_diff>
--- a/sampleFile/book-upload-file.xlsx
+++ b/sampleFile/book-upload-file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishekgautam/Documents/myCode/krishna-book-seller-app/sampleFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936FB14E-C2D1-1942-A5AC-9F96DE6791A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598D5770-0471-6442-85F2-3A3BC96DE70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="980" windowWidth="28040" windowHeight="17440" xr2:uid="{6A18A77D-C05F-9D47-A549-A2705C92245D}"/>
+    <workbookView xWindow="6160" yWindow="1600" windowWidth="28040" windowHeight="17440" xr2:uid="{6A18A77D-C05F-9D47-A549-A2705C92245D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="78">
   <si>
     <t>Ideas C Art &amp; Craft - A</t>
   </si>
@@ -234,6 +234,42 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>six</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>eleven</t>
+  </si>
+  <si>
+    <t>twelve</t>
   </si>
 </sst>
 </file>
@@ -608,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77253596-428E-C34F-88A2-4478B297F427}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" activeCellId="1" sqref="A1:G6 C16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,7 +703,7 @@
         <v>58</v>
       </c>
       <c r="G2" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -690,7 +726,7 @@
         <v>58</v>
       </c>
       <c r="G3" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -713,7 +749,7 @@
         <v>150</v>
       </c>
       <c r="G4" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -736,7 +772,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -759,7 +795,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -790,7 +826,7 @@
         <v>165</v>
       </c>
       <c r="G8" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -813,7 +849,7 @@
         <v>165</v>
       </c>
       <c r="G9" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -836,7 +872,7 @@
         <v>130</v>
       </c>
       <c r="G10" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -859,7 +895,7 @@
         <v>175</v>
       </c>
       <c r="G11" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -882,7 +918,7 @@
         <v>145</v>
       </c>
       <c r="G12" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -905,7 +941,7 @@
         <v>57</v>
       </c>
       <c r="G13" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -928,7 +964,7 @@
         <v>79</v>
       </c>
       <c r="G14" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -951,7 +987,7 @@
         <v>150</v>
       </c>
       <c r="G15" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -974,7 +1010,7 @@
         <v>119</v>
       </c>
       <c r="G16" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -997,7 +1033,7 @@
         <v>150</v>
       </c>
       <c r="G17" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1020,7 +1056,7 @@
         <v>245</v>
       </c>
       <c r="G18" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1043,7 +1079,7 @@
         <v>140</v>
       </c>
       <c r="G19" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1066,7 +1102,7 @@
         <v>250</v>
       </c>
       <c r="G20" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1089,7 +1125,7 @@
         <v>169</v>
       </c>
       <c r="G21" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1120,7 +1156,7 @@
         <v>160</v>
       </c>
       <c r="G23" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1143,7 +1179,7 @@
         <v>165</v>
       </c>
       <c r="G24" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1166,7 +1202,7 @@
         <v>165</v>
       </c>
       <c r="G25" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1189,7 +1225,7 @@
         <v>145</v>
       </c>
       <c r="G26" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1212,7 +1248,7 @@
         <v>57</v>
       </c>
       <c r="G27" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,7 +1271,7 @@
         <v>79</v>
       </c>
       <c r="G28" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1258,7 +1294,7 @@
         <v>150</v>
       </c>
       <c r="G29" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1281,7 +1317,7 @@
         <v>245</v>
       </c>
       <c r="G30" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1304,7 +1340,7 @@
         <v>325</v>
       </c>
       <c r="G31" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1327,7 +1363,7 @@
         <v>150</v>
       </c>
       <c r="G32" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1350,7 +1386,7 @@
         <v>230</v>
       </c>
       <c r="G33" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1373,7 +1409,7 @@
         <v>119</v>
       </c>
       <c r="G34" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1396,7 +1432,7 @@
         <v>165</v>
       </c>
       <c r="G35" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1419,7 +1455,7 @@
         <v>140</v>
       </c>
       <c r="G36" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1450,7 +1486,7 @@
         <v>149</v>
       </c>
       <c r="G38" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1473,7 +1509,7 @@
         <v>165</v>
       </c>
       <c r="G39" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1496,7 +1532,7 @@
         <v>159</v>
       </c>
       <c r="G40" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1519,7 +1555,7 @@
         <v>210</v>
       </c>
       <c r="G41" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1542,7 +1578,7 @@
         <v>160</v>
       </c>
       <c r="G42" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1565,7 +1601,7 @@
         <v>57</v>
       </c>
       <c r="G43" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1588,7 +1624,7 @@
         <v>79</v>
       </c>
       <c r="G44" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1611,7 +1647,7 @@
         <v>245</v>
       </c>
       <c r="G45" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1634,23 +1670,3920 @@
         <v>325</v>
       </c>
       <c r="G46" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D47" s="3"/>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G51" s="3"/>
+      <c r="A48" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="3">
+        <v>150</v>
+      </c>
+      <c r="E48" s="3">
+        <v>120</v>
+      </c>
+      <c r="F48" s="3">
+        <v>160</v>
+      </c>
+      <c r="G48" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3">
+        <v>150</v>
+      </c>
+      <c r="E49" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F49" s="3">
+        <v>165</v>
+      </c>
+      <c r="G49" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="3">
+        <v>150</v>
+      </c>
+      <c r="E50" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F50" s="3">
+        <v>165</v>
+      </c>
+      <c r="G50" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="3">
+        <v>150</v>
+      </c>
+      <c r="E51" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F51" s="3">
+        <v>145</v>
+      </c>
+      <c r="G51" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="3">
+        <v>150</v>
+      </c>
+      <c r="E52" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F52" s="3">
+        <v>57</v>
+      </c>
+      <c r="G52" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="3">
+        <v>150</v>
+      </c>
+      <c r="E53" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F53" s="3">
+        <v>79</v>
+      </c>
+      <c r="G53" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="3">
+        <v>150</v>
+      </c>
+      <c r="E54" s="3">
+        <v>105</v>
+      </c>
+      <c r="F54" s="3">
+        <v>150</v>
+      </c>
+      <c r="G54" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="3">
+        <v>150</v>
+      </c>
+      <c r="E55" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F55" s="3">
+        <v>245</v>
+      </c>
+      <c r="G55" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="3">
+        <v>150</v>
+      </c>
+      <c r="E56" s="3">
+        <v>260</v>
+      </c>
+      <c r="F56" s="3">
+        <v>325</v>
+      </c>
+      <c r="G56" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="3">
+        <v>150</v>
+      </c>
+      <c r="E57" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F57" s="3">
+        <v>150</v>
+      </c>
+      <c r="G57" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="3">
+        <v>150</v>
+      </c>
+      <c r="E58" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F58" s="3">
+        <v>230</v>
+      </c>
+      <c r="G58" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="3">
+        <v>150</v>
+      </c>
+      <c r="E60" s="3">
+        <v>120</v>
+      </c>
+      <c r="F60" s="3">
+        <v>160</v>
+      </c>
+      <c r="G60" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="3">
+        <v>150</v>
+      </c>
+      <c r="E61" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F61" s="3">
+        <v>165</v>
+      </c>
+      <c r="G61" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="3">
+        <v>150</v>
+      </c>
+      <c r="E62" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F62" s="3">
+        <v>165</v>
+      </c>
+      <c r="G62" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="3">
+        <v>150</v>
+      </c>
+      <c r="E63" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F63" s="3">
+        <v>145</v>
+      </c>
+      <c r="G63" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="3">
+        <v>150</v>
+      </c>
+      <c r="E64" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F64" s="3">
+        <v>57</v>
+      </c>
+      <c r="G64" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="3">
+        <v>150</v>
+      </c>
+      <c r="E65" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F65" s="3">
+        <v>79</v>
+      </c>
+      <c r="G65" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="3">
+        <v>150</v>
+      </c>
+      <c r="E66" s="3">
+        <v>105</v>
+      </c>
+      <c r="F66" s="3">
+        <v>150</v>
+      </c>
+      <c r="G66" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="3">
+        <v>150</v>
+      </c>
+      <c r="E67" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F67" s="3">
+        <v>245</v>
+      </c>
+      <c r="G67" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="3">
+        <v>150</v>
+      </c>
+      <c r="E68" s="3">
+        <v>260</v>
+      </c>
+      <c r="F68" s="3">
+        <v>325</v>
+      </c>
+      <c r="G68" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="3">
+        <v>150</v>
+      </c>
+      <c r="E69" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F69" s="3">
+        <v>150</v>
+      </c>
+      <c r="G69" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="3">
+        <v>150</v>
+      </c>
+      <c r="E71" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F71" s="3">
+        <v>119</v>
+      </c>
+      <c r="G71" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="3">
+        <v>150</v>
+      </c>
+      <c r="E72" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F72" s="3">
+        <v>165</v>
+      </c>
+      <c r="G72" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73" s="3">
+        <v>150</v>
+      </c>
+      <c r="E73" s="3">
+        <v>105</v>
+      </c>
+      <c r="F73" s="3">
+        <v>140</v>
+      </c>
+      <c r="G73" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="3">
+        <v>150</v>
+      </c>
+      <c r="E74" s="3">
+        <v>120</v>
+      </c>
+      <c r="F74" s="3">
+        <v>160</v>
+      </c>
+      <c r="G74" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="3">
+        <v>150</v>
+      </c>
+      <c r="E75" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F75" s="3">
+        <v>165</v>
+      </c>
+      <c r="G75" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="3">
+        <v>150</v>
+      </c>
+      <c r="E76" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F76" s="3">
+        <v>165</v>
+      </c>
+      <c r="G76" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="3">
+        <v>150</v>
+      </c>
+      <c r="E77" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F77" s="3">
+        <v>145</v>
+      </c>
+      <c r="G77" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="3">
+        <v>150</v>
+      </c>
+      <c r="E78" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F78" s="3">
+        <v>57</v>
+      </c>
+      <c r="G78" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D79" s="3">
+        <v>150</v>
+      </c>
+      <c r="E79" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F79" s="3">
+        <v>79</v>
+      </c>
+      <c r="G79" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="3">
+        <v>150</v>
+      </c>
+      <c r="E80" s="3">
+        <v>105</v>
+      </c>
+      <c r="F80" s="3">
+        <v>150</v>
+      </c>
+      <c r="G80" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="3">
+        <v>150</v>
+      </c>
+      <c r="E81" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F81" s="3">
+        <v>245</v>
+      </c>
+      <c r="G81" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="3">
+        <v>150</v>
+      </c>
+      <c r="E82" s="3">
+        <v>260</v>
+      </c>
+      <c r="F82" s="3">
+        <v>325</v>
+      </c>
+      <c r="G82" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" s="3">
+        <v>150</v>
+      </c>
+      <c r="E84" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F84" s="3">
+        <v>230</v>
+      </c>
+      <c r="G84" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="3">
+        <v>150</v>
+      </c>
+      <c r="E85" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F85" s="3">
+        <v>119</v>
+      </c>
+      <c r="G85" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="3">
+        <v>150</v>
+      </c>
+      <c r="E86" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F86" s="3">
+        <v>165</v>
+      </c>
+      <c r="G86" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" s="3">
+        <v>150</v>
+      </c>
+      <c r="E87" s="3">
+        <v>105</v>
+      </c>
+      <c r="F87" s="3">
+        <v>140</v>
+      </c>
+      <c r="G87" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="3">
+        <v>150</v>
+      </c>
+      <c r="E88" s="3">
+        <v>120</v>
+      </c>
+      <c r="F88" s="3">
+        <v>160</v>
+      </c>
+      <c r="G88" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="3">
+        <v>150</v>
+      </c>
+      <c r="E89" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F89" s="3">
+        <v>165</v>
+      </c>
+      <c r="G89" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>69</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" s="3">
+        <v>150</v>
+      </c>
+      <c r="E90" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F90" s="3">
+        <v>165</v>
+      </c>
+      <c r="G90" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>69</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="3">
+        <v>150</v>
+      </c>
+      <c r="E91" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F91" s="3">
+        <v>145</v>
+      </c>
+      <c r="G91" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>69</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" s="3">
+        <v>150</v>
+      </c>
+      <c r="E92" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F92" s="3">
+        <v>57</v>
+      </c>
+      <c r="G92" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>69</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" s="3">
+        <v>150</v>
+      </c>
+      <c r="E93" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F93" s="3">
+        <v>79</v>
+      </c>
+      <c r="G93" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>69</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="3">
+        <v>150</v>
+      </c>
+      <c r="E94" s="3">
+        <v>105</v>
+      </c>
+      <c r="F94" s="3">
+        <v>150</v>
+      </c>
+      <c r="G94" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>69</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="3">
+        <v>150</v>
+      </c>
+      <c r="E95" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F95" s="3">
+        <v>245</v>
+      </c>
+      <c r="G95" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D96" s="3">
+        <v>150</v>
+      </c>
+      <c r="E96" s="3">
+        <v>260</v>
+      </c>
+      <c r="F96" s="3">
+        <v>325</v>
+      </c>
+      <c r="G96" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="3">
+        <v>150</v>
+      </c>
+      <c r="E98" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F98" s="3">
+        <v>230</v>
+      </c>
+      <c r="G98" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="3">
+        <v>150</v>
+      </c>
+      <c r="E99" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F99" s="3">
+        <v>119</v>
+      </c>
+      <c r="G99" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" s="3">
+        <v>150</v>
+      </c>
+      <c r="E100" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F100" s="3">
+        <v>165</v>
+      </c>
+      <c r="G100" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101" s="3">
+        <v>150</v>
+      </c>
+      <c r="E101" s="3">
+        <v>105</v>
+      </c>
+      <c r="F101" s="3">
+        <v>140</v>
+      </c>
+      <c r="G101" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" s="3">
+        <v>150</v>
+      </c>
+      <c r="E102" s="3">
+        <v>105</v>
+      </c>
+      <c r="F102" s="3">
+        <v>140</v>
+      </c>
+      <c r="G102" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" s="3">
+        <v>150</v>
+      </c>
+      <c r="E103" s="3">
+        <v>120</v>
+      </c>
+      <c r="F103" s="3">
+        <v>160</v>
+      </c>
+      <c r="G103" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D104" s="3">
+        <v>150</v>
+      </c>
+      <c r="E104" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F104" s="3">
+        <v>165</v>
+      </c>
+      <c r="G104" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="3">
+        <v>150</v>
+      </c>
+      <c r="E105" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F105" s="3">
+        <v>165</v>
+      </c>
+      <c r="G105" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D106" s="3">
+        <v>150</v>
+      </c>
+      <c r="E106" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F106" s="3">
+        <v>145</v>
+      </c>
+      <c r="G106" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="3">
+        <v>150</v>
+      </c>
+      <c r="E107" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F107" s="3">
+        <v>57</v>
+      </c>
+      <c r="G107" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D108" s="3">
+        <v>150</v>
+      </c>
+      <c r="E108" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F108" s="3">
+        <v>79</v>
+      </c>
+      <c r="G108" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D110" s="3">
+        <v>150</v>
+      </c>
+      <c r="E110" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F110" s="3">
+        <v>245</v>
+      </c>
+      <c r="G110" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" s="3">
+        <v>150</v>
+      </c>
+      <c r="E111" s="3">
+        <v>260</v>
+      </c>
+      <c r="F111" s="3">
+        <v>325</v>
+      </c>
+      <c r="G111" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112" s="3">
+        <v>150</v>
+      </c>
+      <c r="E112" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F112" s="3">
+        <v>150</v>
+      </c>
+      <c r="G112" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D113" s="3">
+        <v>150</v>
+      </c>
+      <c r="E113" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F113" s="3">
+        <v>230</v>
+      </c>
+      <c r="G113" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114" s="3">
+        <v>150</v>
+      </c>
+      <c r="E114" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F114" s="3">
+        <v>119</v>
+      </c>
+      <c r="G114" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" s="3">
+        <v>150</v>
+      </c>
+      <c r="E115" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F115" s="3">
+        <v>165</v>
+      </c>
+      <c r="G115" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D116" s="3">
+        <v>150</v>
+      </c>
+      <c r="E116" s="3">
+        <v>105</v>
+      </c>
+      <c r="F116" s="3">
+        <v>140</v>
+      </c>
+      <c r="G116" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="3">
+        <v>150</v>
+      </c>
+      <c r="E117" s="3">
+        <v>120</v>
+      </c>
+      <c r="F117" s="3">
+        <v>160</v>
+      </c>
+      <c r="G117" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D118" s="3">
+        <v>150</v>
+      </c>
+      <c r="E118" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F118" s="3">
+        <v>165</v>
+      </c>
+      <c r="G118" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" s="3">
+        <v>150</v>
+      </c>
+      <c r="E119" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F119" s="3">
+        <v>165</v>
+      </c>
+      <c r="G119" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" s="3">
+        <v>150</v>
+      </c>
+      <c r="E120" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F120" s="3">
+        <v>145</v>
+      </c>
+      <c r="G120" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D121" s="3">
+        <v>150</v>
+      </c>
+      <c r="E121" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F121" s="3">
+        <v>57</v>
+      </c>
+      <c r="G121" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="3">
+        <v>150</v>
+      </c>
+      <c r="E122" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F122" s="3">
+        <v>79</v>
+      </c>
+      <c r="G122" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D124" s="3">
+        <v>150</v>
+      </c>
+      <c r="E124" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F124" s="3">
+        <v>245</v>
+      </c>
+      <c r="G124" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125" s="3">
+        <v>150</v>
+      </c>
+      <c r="E125" s="3">
+        <v>260</v>
+      </c>
+      <c r="F125" s="3">
+        <v>325</v>
+      </c>
+      <c r="G125" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D126" s="3">
+        <v>150</v>
+      </c>
+      <c r="E126" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F126" s="3">
+        <v>150</v>
+      </c>
+      <c r="G126" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D127" s="3">
+        <v>150</v>
+      </c>
+      <c r="E127" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F127" s="3">
+        <v>230</v>
+      </c>
+      <c r="G127" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" s="3">
+        <v>150</v>
+      </c>
+      <c r="E128" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F128" s="3">
+        <v>119</v>
+      </c>
+      <c r="G128" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" s="3">
+        <v>150</v>
+      </c>
+      <c r="E129" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F129" s="3">
+        <v>165</v>
+      </c>
+      <c r="G129" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130" s="3">
+        <v>150</v>
+      </c>
+      <c r="E130" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F130" s="3">
+        <v>165</v>
+      </c>
+      <c r="G130" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" s="3">
+        <v>150</v>
+      </c>
+      <c r="E131" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F131" s="3">
+        <v>165</v>
+      </c>
+      <c r="G131" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D132" s="3">
+        <v>150</v>
+      </c>
+      <c r="E132" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F132" s="3">
+        <v>145</v>
+      </c>
+      <c r="G132" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D133" s="3">
+        <v>150</v>
+      </c>
+      <c r="E133" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F133" s="3">
+        <v>57</v>
+      </c>
+      <c r="G133" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D134" s="3">
+        <v>150</v>
+      </c>
+      <c r="E134" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F134" s="3">
+        <v>79</v>
+      </c>
+      <c r="G134" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D135" s="3">
+        <v>150</v>
+      </c>
+      <c r="E135" s="3">
+        <v>105</v>
+      </c>
+      <c r="F135" s="3">
+        <v>150</v>
+      </c>
+      <c r="G135" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" s="3">
+        <v>150</v>
+      </c>
+      <c r="E136" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F136" s="3">
+        <v>245</v>
+      </c>
+      <c r="G136" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="3">
+        <v>150</v>
+      </c>
+      <c r="E137" s="3">
+        <v>260</v>
+      </c>
+      <c r="F137" s="3">
+        <v>325</v>
+      </c>
+      <c r="G137" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>73</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" s="3">
+        <v>150</v>
+      </c>
+      <c r="E139" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F139" s="3">
+        <v>230</v>
+      </c>
+      <c r="G139" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>73</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D140" s="3">
+        <v>150</v>
+      </c>
+      <c r="E140" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F140" s="3">
+        <v>119</v>
+      </c>
+      <c r="G140" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>73</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D141" s="3">
+        <v>150</v>
+      </c>
+      <c r="E141" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F141" s="3">
+        <v>165</v>
+      </c>
+      <c r="G141" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>73</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D142" s="3">
+        <v>150</v>
+      </c>
+      <c r="E142" s="3">
+        <v>105</v>
+      </c>
+      <c r="F142" s="3">
+        <v>140</v>
+      </c>
+      <c r="G142" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>73</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D143" s="3">
+        <v>150</v>
+      </c>
+      <c r="E143" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F143" s="3">
+        <v>230</v>
+      </c>
+      <c r="G143" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>73</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D144" s="3">
+        <v>150</v>
+      </c>
+      <c r="E144" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F144" s="3">
+        <v>119</v>
+      </c>
+      <c r="G144" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>73</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D145" s="3">
+        <v>150</v>
+      </c>
+      <c r="E145" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F145" s="3">
+        <v>165</v>
+      </c>
+      <c r="G145" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>73</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="3">
+        <v>150</v>
+      </c>
+      <c r="E146" s="3">
+        <v>105</v>
+      </c>
+      <c r="F146" s="3">
+        <v>140</v>
+      </c>
+      <c r="G146" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>73</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D147" s="3">
+        <v>150</v>
+      </c>
+      <c r="E147" s="3">
+        <v>120</v>
+      </c>
+      <c r="F147" s="3">
+        <v>160</v>
+      </c>
+      <c r="G147" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>73</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D148" s="3">
+        <v>150</v>
+      </c>
+      <c r="E148" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F148" s="3">
+        <v>165</v>
+      </c>
+      <c r="G148" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>73</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D149" s="3">
+        <v>150</v>
+      </c>
+      <c r="E149" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F149" s="3">
+        <v>165</v>
+      </c>
+      <c r="G149" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>73</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D150" s="3">
+        <v>150</v>
+      </c>
+      <c r="E150" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F150" s="3">
+        <v>145</v>
+      </c>
+      <c r="G150" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>73</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151" s="3">
+        <v>150</v>
+      </c>
+      <c r="E151" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F151" s="3">
+        <v>57</v>
+      </c>
+      <c r="G151" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>73</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D152" s="3">
+        <v>150</v>
+      </c>
+      <c r="E152" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F152" s="3">
+        <v>79</v>
+      </c>
+      <c r="G152" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>73</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D153" s="3">
+        <v>150</v>
+      </c>
+      <c r="E153" s="3">
+        <v>105</v>
+      </c>
+      <c r="F153" s="3">
+        <v>150</v>
+      </c>
+      <c r="G153" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D155" s="3">
+        <v>150</v>
+      </c>
+      <c r="E155" s="3">
+        <v>260</v>
+      </c>
+      <c r="F155" s="3">
+        <v>325</v>
+      </c>
+      <c r="G155" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" s="3">
+        <v>150</v>
+      </c>
+      <c r="E156" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F156" s="3">
+        <v>150</v>
+      </c>
+      <c r="G156" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D157" s="3">
+        <v>150</v>
+      </c>
+      <c r="E157" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F157" s="3">
+        <v>230</v>
+      </c>
+      <c r="G157" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D158" s="3">
+        <v>150</v>
+      </c>
+      <c r="E158" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F158" s="3">
+        <v>119</v>
+      </c>
+      <c r="G158" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D159" s="3">
+        <v>150</v>
+      </c>
+      <c r="E159" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F159" s="3">
+        <v>165</v>
+      </c>
+      <c r="G159" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D160" s="3">
+        <v>150</v>
+      </c>
+      <c r="E160" s="3">
+        <v>105</v>
+      </c>
+      <c r="F160" s="3">
+        <v>140</v>
+      </c>
+      <c r="G160" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D161" s="3">
+        <v>150</v>
+      </c>
+      <c r="E161" s="3">
+        <v>105</v>
+      </c>
+      <c r="F161" s="3">
+        <v>140</v>
+      </c>
+      <c r="G161" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" s="3">
+        <v>150</v>
+      </c>
+      <c r="E162" s="3">
+        <v>120</v>
+      </c>
+      <c r="F162" s="3">
+        <v>160</v>
+      </c>
+      <c r="G162" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D163" s="3">
+        <v>150</v>
+      </c>
+      <c r="E163" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F163" s="3">
+        <v>165</v>
+      </c>
+      <c r="G163" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D164" s="3">
+        <v>150</v>
+      </c>
+      <c r="E164" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F164" s="3">
+        <v>165</v>
+      </c>
+      <c r="G164" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D165" s="3">
+        <v>150</v>
+      </c>
+      <c r="E165" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F165" s="3">
+        <v>145</v>
+      </c>
+      <c r="G165" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D166" s="3">
+        <v>150</v>
+      </c>
+      <c r="E166" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F166" s="3">
+        <v>57</v>
+      </c>
+      <c r="G166" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D167" s="3">
+        <v>150</v>
+      </c>
+      <c r="E167" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F167" s="3">
+        <v>79</v>
+      </c>
+      <c r="G167" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D168" s="3">
+        <v>150</v>
+      </c>
+      <c r="E168" s="3">
+        <v>105</v>
+      </c>
+      <c r="F168" s="3">
+        <v>150</v>
+      </c>
+      <c r="G168" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D169" s="3">
+        <v>150</v>
+      </c>
+      <c r="E169" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F169" s="3">
+        <v>245</v>
+      </c>
+      <c r="G169" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C170" s="3"/>
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D171" s="3">
+        <v>150</v>
+      </c>
+      <c r="E171" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F171" s="3">
+        <v>150</v>
+      </c>
+      <c r="G171" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D172" s="3">
+        <v>150</v>
+      </c>
+      <c r="E172" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F172" s="3">
+        <v>230</v>
+      </c>
+      <c r="G172" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D173" s="3">
+        <v>150</v>
+      </c>
+      <c r="E173" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F173" s="3">
+        <v>119</v>
+      </c>
+      <c r="G173" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D174" s="3">
+        <v>150</v>
+      </c>
+      <c r="E174" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F174" s="3">
+        <v>165</v>
+      </c>
+      <c r="G174" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D175" s="3">
+        <v>150</v>
+      </c>
+      <c r="E175" s="3">
+        <v>105</v>
+      </c>
+      <c r="F175" s="3">
+        <v>140</v>
+      </c>
+      <c r="G175" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D176" s="3">
+        <v>150</v>
+      </c>
+      <c r="E176" s="3">
+        <v>120</v>
+      </c>
+      <c r="F176" s="3">
+        <v>160</v>
+      </c>
+      <c r="G176" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D177" s="3">
+        <v>150</v>
+      </c>
+      <c r="E177" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F177" s="3">
+        <v>165</v>
+      </c>
+      <c r="G177" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D178" s="3">
+        <v>150</v>
+      </c>
+      <c r="E178" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F178" s="3">
+        <v>165</v>
+      </c>
+      <c r="G178" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D179" s="3">
+        <v>150</v>
+      </c>
+      <c r="E179" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F179" s="3">
+        <v>145</v>
+      </c>
+      <c r="G179" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D180" s="3">
+        <v>150</v>
+      </c>
+      <c r="E180" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F180" s="3">
+        <v>57</v>
+      </c>
+      <c r="G180" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" s="3">
+        <v>150</v>
+      </c>
+      <c r="E181" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F181" s="3">
+        <v>79</v>
+      </c>
+      <c r="G181" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D182" s="3">
+        <v>150</v>
+      </c>
+      <c r="E182" s="3">
+        <v>105</v>
+      </c>
+      <c r="F182" s="3">
+        <v>150</v>
+      </c>
+      <c r="G182" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D183" s="3">
+        <v>150</v>
+      </c>
+      <c r="E183" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F183" s="3">
+        <v>245</v>
+      </c>
+      <c r="G183" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D184" s="3">
+        <v>150</v>
+      </c>
+      <c r="E184" s="3">
+        <v>260</v>
+      </c>
+      <c r="F184" s="3">
+        <v>325</v>
+      </c>
+      <c r="G184" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D185" s="3">
+        <v>150</v>
+      </c>
+      <c r="E185" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F185" s="3">
+        <v>150</v>
+      </c>
+      <c r="G185" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D186" s="3">
+        <v>150</v>
+      </c>
+      <c r="E186" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F186" s="3">
+        <v>230</v>
+      </c>
+      <c r="G186" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="3">
+        <v>150</v>
+      </c>
+      <c r="E187" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F187" s="3">
+        <v>119</v>
+      </c>
+      <c r="G187" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D189" s="3">
+        <v>150</v>
+      </c>
+      <c r="E189" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F189" s="3">
+        <v>165</v>
+      </c>
+      <c r="G189" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D190" s="3">
+        <v>150</v>
+      </c>
+      <c r="E190" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F190" s="3">
+        <v>165</v>
+      </c>
+      <c r="G190" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D191" s="3">
+        <v>150</v>
+      </c>
+      <c r="E191" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F191" s="3">
+        <v>145</v>
+      </c>
+      <c r="G191" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D192" s="3">
+        <v>150</v>
+      </c>
+      <c r="E192" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F192" s="3">
+        <v>57</v>
+      </c>
+      <c r="G192" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A193" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D193" s="3">
+        <v>150</v>
+      </c>
+      <c r="E193" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F193" s="3">
+        <v>79</v>
+      </c>
+      <c r="G193" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D194" s="3">
+        <v>150</v>
+      </c>
+      <c r="E194" s="3">
+        <v>105</v>
+      </c>
+      <c r="F194" s="3">
+        <v>150</v>
+      </c>
+      <c r="G194" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A195" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D195" s="3">
+        <v>150</v>
+      </c>
+      <c r="E195" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F195" s="3">
+        <v>245</v>
+      </c>
+      <c r="G195" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A196" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" s="3">
+        <v>150</v>
+      </c>
+      <c r="E196" s="3">
+        <v>260</v>
+      </c>
+      <c r="F196" s="3">
+        <v>325</v>
+      </c>
+      <c r="G196" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A197" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D197" s="3">
+        <v>150</v>
+      </c>
+      <c r="E197" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F197" s="3">
+        <v>150</v>
+      </c>
+      <c r="G197" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D198" s="3">
+        <v>150</v>
+      </c>
+      <c r="E198" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F198" s="3">
+        <v>230</v>
+      </c>
+      <c r="G198" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D199" s="3">
+        <v>150</v>
+      </c>
+      <c r="E199" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F199" s="3">
+        <v>119</v>
+      </c>
+      <c r="G199" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D200" s="3">
+        <v>150</v>
+      </c>
+      <c r="E200" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F200" s="3">
+        <v>165</v>
+      </c>
+      <c r="G200" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A201" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D201" s="3">
+        <v>150</v>
+      </c>
+      <c r="E201" s="3">
+        <v>105</v>
+      </c>
+      <c r="F201" s="3">
+        <v>140</v>
+      </c>
+      <c r="G201" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B202" s="3"/>
+      <c r="D202" s="3"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>77</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D203" s="3">
+        <v>150</v>
+      </c>
+      <c r="E203" s="3">
+        <v>105</v>
+      </c>
+      <c r="F203" s="3">
+        <v>150</v>
+      </c>
+      <c r="G203" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>77</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D204" s="3">
+        <v>150</v>
+      </c>
+      <c r="E204" s="3">
+        <v>183.75</v>
+      </c>
+      <c r="F204" s="3">
+        <v>245</v>
+      </c>
+      <c r="G204" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>77</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D205" s="3">
+        <v>150</v>
+      </c>
+      <c r="E205" s="3">
+        <v>260</v>
+      </c>
+      <c r="F205" s="3">
+        <v>325</v>
+      </c>
+      <c r="G205" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>77</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D206" s="3">
+        <v>150</v>
+      </c>
+      <c r="E206" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="F206" s="3">
+        <v>150</v>
+      </c>
+      <c r="G206" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>77</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D207" s="3">
+        <v>150</v>
+      </c>
+      <c r="E207" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="F207" s="3">
+        <v>230</v>
+      </c>
+      <c r="G207" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>77</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D208" s="3">
+        <v>150</v>
+      </c>
+      <c r="E208" s="3">
+        <v>89.25</v>
+      </c>
+      <c r="F208" s="3">
+        <v>119</v>
+      </c>
+      <c r="G208" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>77</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D209" s="3">
+        <v>150</v>
+      </c>
+      <c r="E209" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F209" s="3">
+        <v>165</v>
+      </c>
+      <c r="G209" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>77</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D210" s="3">
+        <v>150</v>
+      </c>
+      <c r="E210" s="3">
+        <v>105</v>
+      </c>
+      <c r="F210" s="3">
+        <v>140</v>
+      </c>
+      <c r="G210" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>77</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D211" s="3">
+        <v>150</v>
+      </c>
+      <c r="E211" s="3">
+        <v>105</v>
+      </c>
+      <c r="F211" s="3">
+        <v>140</v>
+      </c>
+      <c r="G211" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>77</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D212" s="3">
+        <v>150</v>
+      </c>
+      <c r="E212" s="3">
+        <v>120</v>
+      </c>
+      <c r="F212" s="3">
+        <v>160</v>
+      </c>
+      <c r="G212" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>77</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D213" s="3">
+        <v>150</v>
+      </c>
+      <c r="E213" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F213" s="3">
+        <v>165</v>
+      </c>
+      <c r="G213" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>77</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D214" s="3">
+        <v>150</v>
+      </c>
+      <c r="E214" s="3">
+        <v>123.75</v>
+      </c>
+      <c r="F214" s="3">
+        <v>165</v>
+      </c>
+      <c r="G214" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>77</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D215" s="3">
+        <v>150</v>
+      </c>
+      <c r="E215" s="3">
+        <v>108.75</v>
+      </c>
+      <c r="F215" s="3">
+        <v>145</v>
+      </c>
+      <c r="G215" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>77</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D216" s="3">
+        <v>150</v>
+      </c>
+      <c r="E216" s="3">
+        <v>30.4</v>
+      </c>
+      <c r="F216" s="3">
+        <v>57</v>
+      </c>
+      <c r="G216" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>77</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D217" s="3">
+        <v>150</v>
+      </c>
+      <c r="E217" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="F217" s="3">
+        <v>79</v>
+      </c>
+      <c r="G217" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B218" s="3"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="3"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B219" s="3"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
+    </row>
+    <row r="225" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
+    </row>
+    <row r="226" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+    </row>
+    <row r="227" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E227" s="3"/>
+      <c r="F227" s="3"/>
+      <c r="G227" s="3"/>
+    </row>
+    <row r="228" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E228" s="3"/>
+      <c r="F228" s="3"/>
+      <c r="G228" s="3"/>
+    </row>
+    <row r="229" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E229" s="3"/>
+      <c r="F229" s="3"/>
+      <c r="G229" s="3"/>
+    </row>
+    <row r="230" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E230" s="3"/>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
+    </row>
+    <row r="231" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
+    </row>
+    <row r="232" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
+    </row>
+    <row r="233" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
+    </row>
+    <row r="234" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+      <c r="G234" s="3"/>
+    </row>
+    <row r="235" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+    </row>
+    <row r="236" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
+    </row>
+    <row r="237" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
+    </row>
+    <row r="238" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
+    </row>
+    <row r="239" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="3"/>
+    </row>
+    <row r="240" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="3"/>
+    </row>
+    <row r="241" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="3"/>
+    </row>
+    <row r="242" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
+    </row>
+    <row r="243" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="3"/>
+    </row>
+    <row r="244" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
+    </row>
+    <row r="245" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="3"/>
+    </row>
+    <row r="246" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="3"/>
+    </row>
+    <row r="247" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="3"/>
+    </row>
+    <row r="248" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="3"/>
+    </row>
+    <row r="249" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
+    </row>
+    <row r="250" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
+    </row>
+    <row r="251" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>